<commit_message>
yay enemies shoot at me
</commit_message>
<xml_diff>
--- a/Pinto_Tomas_NuclearMiami/Pinto_Tomas_NuclearMiami/Pinto_Tomas_NuclearMiami.xlsx
+++ b/Pinto_Tomas_NuclearMiami/Pinto_Tomas_NuclearMiami/Pinto_Tomas_NuclearMiami.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2018_2019\_Programming2\00_GameProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositories\1DAE_PROG_FINAL\Pinto_Tomas_NuclearMiami\Pinto_Tomas_NuclearMiami\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD12E1CC-3B2A-4282-A02F-23D599612F08}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8472"/>
+    <workbookView xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Game play description" sheetId="4" r:id="rId1"/>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="52">
   <si>
     <t>Topic</t>
   </si>
@@ -130,76 +131,73 @@
     <t>Level</t>
   </si>
   <si>
-    <t xml:space="preserve">The  level is divided into several maps, each of which is completed when Rayman reaches the "!" sign at the end. </t>
-  </si>
-  <si>
     <t>Lives</t>
   </si>
   <si>
-    <t xml:space="preserve">The player is given a certain number of lives, which are lost when Rayman takes too many hits or falls into water or a pit. 
-If all lives are lost at any point, the "Game Over" screen will appear.
-Scattered around the level are small, sparkling blue spheres called Tings.
- If the player controlling Rayman picks up 100 (50 in the DSi version), he gains an extra life and the counter resets to zero. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">At the end of the level, Rayman must defeat a boss enemy. </t>
-  </si>
-  <si>
     <t>Boss enemy</t>
   </si>
   <si>
-    <t>The player comes across a variety of other power-ups and bonuses, such as a golden fist (which increases punch strength), a speed fist (which increases the speed of Rayman's punches), a power to restore Rayman's lost life energy, and flying blue elves whose touch shrinks Rayman down in size to access new areas.</t>
-  </si>
-  <si>
     <t>Game part</t>
   </si>
   <si>
     <t>Description</t>
   </si>
   <si>
-    <t xml:space="preserve">The player character is Rayman, who must travel through the level to free all of the caged Electoons. 
+    <t>Power-ups</t>
+  </si>
+  <si>
+    <t>Enemies</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>…</t>
+  </si>
+  <si>
+    <t>Enemies are drawn at the right position in the level</t>
+  </si>
+  <si>
+    <t>Enemies perform their animations and move correctly</t>
+  </si>
+  <si>
+    <t>Power-ups are drawn at the right position in the level</t>
+  </si>
+  <si>
+    <t>Power-ups perform their animations and move correctly</t>
+  </si>
+  <si>
+    <t>Interaction player enemies</t>
+  </si>
+  <si>
+    <t>The game is a mix of Nuclear Throne with Hotline Miami, both of these are topdown fastpaced shooter games.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The player backstory is still no decided.
 </t>
   </si>
   <si>
-    <t>Power-ups</t>
-  </si>
-  <si>
-    <t>Enemies</t>
-  </si>
-  <si>
-    <t>General</t>
-  </si>
-  <si>
-    <t>The Great Protoon maintains peace and balance throughout a valley that is Rayman's world. 
-One day, the evil Mr. Dark steals the Great Protoon, leaving the Electoons, small beings who gravitate around it, vulnerable to Mr. Dark's forces, who have captured the Electoons in cages. 
-Rayman must free the Electoons and recover the Great Protoon to restore the valley's balance. 
-Betilla the Fairy, a guardian of the Great Protoon, frequently interacts with Rayman as needed to give him additional magical powers along his journey.</t>
-  </si>
-  <si>
-    <t>…</t>
-  </si>
-  <si>
-    <t>Enemies are drawn at the right position in the level</t>
-  </si>
-  <si>
-    <t>Enemies perform their animations and move correctly</t>
-  </si>
-  <si>
-    <t>Power-ups are drawn at the right position in the level</t>
-  </si>
-  <si>
-    <t>Power-ups perform their animations and move correctly</t>
-  </si>
-  <si>
-    <t>Interaction player enemies</t>
+    <t>In the game, for each level you spawn in an initial room with basic weaponry. He collects new weapons from the level as he progressed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The exact ammount of health is not yet decided but it will be low, this so to provide a sense of challenge. </t>
+  </si>
+  <si>
+    <t>There will be multiple different sorts of enemies, Melee, With simple weaponry, with more complex weaponry, and finally the boss with a rare weapon that you can take to the next level</t>
+  </si>
+  <si>
+    <t>When it comes to power ups, it will mostly be health(med kits). Not decided yet.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">At the end of each level there are stronger versions of the enemies, these are bosses. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="[$-409]d\-mmm\-yy;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -309,11 +307,11 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Kop 1" xfId="1" builtinId="16"/>
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="7">
     <dxf>
@@ -645,119 +643,116 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B12" sqref="B12"/>
+      <selection pane="bottomRight" activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.88671875" customWidth="1"/>
-    <col min="2" max="2" width="206.33203125" customWidth="1"/>
+    <col min="1" max="1" width="27.85546875" customWidth="1"/>
+    <col min="2" max="2" width="206.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="81" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
-        <v>43</v>
-      </c>
       <c r="B2" s="5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>30</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="16.2" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>31</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" ht="64.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+      <c r="B5" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="32.4" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
+      <c r="B6" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="32.4" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
-        <v>41</v>
-      </c>
       <c r="B7" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
-        <v>42</v>
-      </c>
       <c r="B8" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="16.2" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" location="cite_note-atarimanual6-3" display="https://en.wikipedia.org/wiki/Rayman_(video_game) - cite_note-atarimanual6-3"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E24" sqref="E24"/>
+      <selection pane="bottomRight" activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -771,7 +766,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="21.6" thickTop="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:4" ht="21.75" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>12</v>
       </c>
@@ -779,7 +774,7 @@
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -793,7 +788,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -807,7 +802,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>16</v>
       </c>
@@ -815,7 +810,7 @@
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -826,7 +821,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -837,7 +832,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="21" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>13</v>
       </c>
@@ -845,7 +840,7 @@
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -859,7 +854,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -870,7 +865,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -884,7 +879,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="21" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>21</v>
       </c>
@@ -892,7 +887,7 @@
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -904,7 +899,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:D1"/>
+  <autoFilter ref="B1:D1" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <conditionalFormatting sqref="C1:C1048576">
     <cfRule type="containsText" dxfId="6" priority="27" operator="containsText" text="Finished">
       <formula>NOT(ISERROR(SEARCH("Finished",C1)))</formula>
@@ -933,10 +928,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B7 B9:B11 B13">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B7 B9:B11 B13" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Low,Medium,High"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C13">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C13" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"Not started,WIP,Finished"</formula1>
     </dataValidation>
   </dataValidations>
@@ -946,21 +941,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
+      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="65.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="65.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>23</v>
       </c>
@@ -968,7 +963,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>25</v>
       </c>
@@ -976,7 +971,7 @@
         <v>43528</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>22</v>
       </c>
@@ -986,7 +981,7 @@
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>26</v>
       </c>
@@ -996,7 +991,7 @@
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>27</v>
       </c>
@@ -1006,9 +1001,9 @@
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B6" s="8">
         <v>43538</v>
@@ -1016,297 +1011,297 @@
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
     </row>
-    <row r="17" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
     </row>
-    <row r="22" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
     </row>
-    <row r="23" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
     </row>
-    <row r="24" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
     </row>
-    <row r="26" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="7"/>
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
     </row>
-    <row r="27" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
       <c r="B27" s="7"/>
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
     </row>
-    <row r="28" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
     </row>
-    <row r="29" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="7"/>
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
     </row>
-    <row r="30" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
     </row>
-    <row r="31" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
     </row>
-    <row r="32" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
     </row>
-    <row r="33" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="7"/>
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
       <c r="D33" s="7"/>
     </row>
-    <row r="34" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
       <c r="B34" s="7"/>
       <c r="C34" s="7"/>
       <c r="D34" s="7"/>
     </row>
-    <row r="35" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="7"/>
       <c r="B35" s="7"/>
       <c r="C35" s="7"/>
       <c r="D35" s="7"/>
     </row>
-    <row r="36" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="7"/>
       <c r="B36" s="7"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
     </row>
-    <row r="37" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
       <c r="B37" s="7"/>
       <c r="C37" s="7"/>
       <c r="D37" s="7"/>
     </row>
-    <row r="38" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="7"/>
       <c r="B38" s="7"/>
       <c r="C38" s="7"/>
       <c r="D38" s="7"/>
     </row>
-    <row r="39" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="7"/>
       <c r="B39" s="7"/>
       <c r="C39" s="7"/>
       <c r="D39" s="7"/>
     </row>
-    <row r="40" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
       <c r="B40" s="7"/>
       <c r="C40" s="7"/>
       <c r="D40" s="7"/>
     </row>
-    <row r="41" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
       <c r="B41" s="7"/>
       <c r="C41" s="7"/>
       <c r="D41" s="7"/>
     </row>
-    <row r="42" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="7"/>
       <c r="B42" s="7"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
     </row>
-    <row r="43" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="7"/>
       <c r="B43" s="7"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
     </row>
-    <row r="44" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="7"/>
       <c r="B44" s="7"/>
       <c r="C44" s="7"/>
       <c r="D44" s="7"/>
     </row>
-    <row r="45" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="7"/>
       <c r="B45" s="7"/>
       <c r="C45" s="7"/>
       <c r="D45" s="7"/>
     </row>
-    <row r="46" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="7"/>
       <c r="B46" s="7"/>
       <c r="C46" s="7"/>
       <c r="D46" s="7"/>
     </row>
-    <row r="47" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="7"/>
       <c r="B47" s="7"/>
       <c r="C47" s="7"/>
       <c r="D47" s="7"/>
     </row>
-    <row r="48" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="7"/>
       <c r="B48" s="7"/>
       <c r="C48" s="7"/>
       <c r="D48" s="7"/>
     </row>
-    <row r="49" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="7"/>
       <c r="B49" s="7"/>
       <c r="C49" s="7"/>
       <c r="D49" s="7"/>
     </row>
-    <row r="50" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="7"/>
       <c r="B50" s="7"/>
       <c r="C50" s="7"/>
       <c r="D50" s="7"/>
     </row>
-    <row r="51" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="7"/>
       <c r="B51" s="7"/>
       <c r="C51" s="7"/>
       <c r="D51" s="7"/>
     </row>
-    <row r="52" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="7"/>
       <c r="B52" s="7"/>
       <c r="C52" s="7"/>
       <c r="D52" s="7"/>
     </row>
-    <row r="53" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="7"/>
       <c r="B53" s="7"/>
       <c r="C53" s="7"/>
       <c r="D53" s="7"/>
     </row>
-    <row r="54" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="7"/>
       <c r="B54" s="7"/>
       <c r="C54" s="7"/>
       <c r="D54" s="7"/>
     </row>
-    <row r="55" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="7"/>
       <c r="B55" s="7"/>
       <c r="C55" s="7"/>
@@ -1318,7 +1313,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1326,300 +1321,300 @@
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="65.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="65.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>22</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
     </row>
-    <row r="4" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>26</v>
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
     </row>
-    <row r="5" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>27</v>
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
     </row>
-    <row r="6" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
     </row>
-    <row r="7" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
     </row>
-    <row r="8" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
     </row>
-    <row r="9" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
     </row>
-    <row r="10" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
     </row>
-    <row r="11" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
     </row>
-    <row r="12" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
     </row>
-    <row r="13" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
     </row>
-    <row r="14" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
     </row>
-    <row r="15" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
     </row>
-    <row r="16" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
     </row>
-    <row r="17" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
     </row>
-    <row r="18" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
     </row>
-    <row r="19" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
     </row>
-    <row r="20" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
     </row>
-    <row r="21" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
     </row>
-    <row r="22" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
     </row>
-    <row r="23" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
     </row>
-    <row r="24" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
     </row>
-    <row r="25" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
     </row>
-    <row r="26" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="7"/>
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
     </row>
-    <row r="27" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
       <c r="B27" s="7"/>
       <c r="C27" s="7"/>
     </row>
-    <row r="28" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
     </row>
-    <row r="29" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="7"/>
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
     </row>
-    <row r="30" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
     </row>
-    <row r="31" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
     </row>
-    <row r="32" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
     </row>
-    <row r="33" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="7"/>
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
     </row>
-    <row r="34" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
       <c r="B34" s="7"/>
       <c r="C34" s="7"/>
     </row>
-    <row r="35" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="7"/>
       <c r="B35" s="7"/>
       <c r="C35" s="7"/>
     </row>
-    <row r="36" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="7"/>
       <c r="B36" s="7"/>
       <c r="C36" s="7"/>
     </row>
-    <row r="37" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
       <c r="B37" s="7"/>
       <c r="C37" s="7"/>
     </row>
-    <row r="38" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="7"/>
       <c r="B38" s="7"/>
       <c r="C38" s="7"/>
     </row>
-    <row r="39" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="7"/>
       <c r="B39" s="7"/>
       <c r="C39" s="7"/>
     </row>
-    <row r="40" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
       <c r="B40" s="7"/>
       <c r="C40" s="7"/>
     </row>
-    <row r="41" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
       <c r="B41" s="7"/>
       <c r="C41" s="7"/>
     </row>
-    <row r="42" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="7"/>
       <c r="B42" s="7"/>
       <c r="C42" s="7"/>
     </row>
-    <row r="43" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="7"/>
       <c r="B43" s="7"/>
       <c r="C43" s="7"/>
     </row>
-    <row r="44" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="7"/>
       <c r="B44" s="7"/>
       <c r="C44" s="7"/>
     </row>
-    <row r="45" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="7"/>
       <c r="B45" s="7"/>
       <c r="C45" s="7"/>
     </row>
-    <row r="46" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="7"/>
       <c r="B46" s="7"/>
       <c r="C46" s="7"/>
     </row>
-    <row r="47" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="7"/>
       <c r="B47" s="7"/>
       <c r="C47" s="7"/>
     </row>
-    <row r="48" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="7"/>
       <c r="B48" s="7"/>
       <c r="C48" s="7"/>
     </row>
-    <row r="49" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="7"/>
       <c r="B49" s="7"/>
       <c r="C49" s="7"/>
     </row>
-    <row r="50" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="7"/>
       <c r="B50" s="7"/>
       <c r="C50" s="7"/>
     </row>
-    <row r="51" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="7"/>
       <c r="B51" s="7"/>
       <c r="C51" s="7"/>
     </row>
-    <row r="52" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="7"/>
       <c r="B52" s="7"/>
       <c r="C52" s="7"/>
     </row>
-    <row r="53" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="7"/>
       <c r="B53" s="7"/>
       <c r="C53" s="7"/>
     </row>
-    <row r="54" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="7"/>
       <c r="B54" s="7"/>
       <c r="C54" s="7"/>
     </row>
-    <row r="55" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="7"/>
       <c r="B55" s="7"/>
       <c r="C55" s="7"/>
@@ -1630,7 +1625,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1638,300 +1633,300 @@
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="65.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="65.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>22</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
     </row>
-    <row r="4" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>26</v>
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
     </row>
-    <row r="5" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>27</v>
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
     </row>
-    <row r="6" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
     </row>
-    <row r="7" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
     </row>
-    <row r="8" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
     </row>
-    <row r="9" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
     </row>
-    <row r="10" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
     </row>
-    <row r="11" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
     </row>
-    <row r="12" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
     </row>
-    <row r="13" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
     </row>
-    <row r="14" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
     </row>
-    <row r="15" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
     </row>
-    <row r="16" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
     </row>
-    <row r="17" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
     </row>
-    <row r="18" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
     </row>
-    <row r="19" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
     </row>
-    <row r="20" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
     </row>
-    <row r="21" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
     </row>
-    <row r="22" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
     </row>
-    <row r="23" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
     </row>
-    <row r="24" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
     </row>
-    <row r="25" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
     </row>
-    <row r="26" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="7"/>
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
     </row>
-    <row r="27" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
       <c r="B27" s="7"/>
       <c r="C27" s="7"/>
     </row>
-    <row r="28" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
     </row>
-    <row r="29" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="7"/>
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
     </row>
-    <row r="30" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
     </row>
-    <row r="31" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
     </row>
-    <row r="32" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
     </row>
-    <row r="33" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="7"/>
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
     </row>
-    <row r="34" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
       <c r="B34" s="7"/>
       <c r="C34" s="7"/>
     </row>
-    <row r="35" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="7"/>
       <c r="B35" s="7"/>
       <c r="C35" s="7"/>
     </row>
-    <row r="36" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="7"/>
       <c r="B36" s="7"/>
       <c r="C36" s="7"/>
     </row>
-    <row r="37" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
       <c r="B37" s="7"/>
       <c r="C37" s="7"/>
     </row>
-    <row r="38" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="7"/>
       <c r="B38" s="7"/>
       <c r="C38" s="7"/>
     </row>
-    <row r="39" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="7"/>
       <c r="B39" s="7"/>
       <c r="C39" s="7"/>
     </row>
-    <row r="40" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
       <c r="B40" s="7"/>
       <c r="C40" s="7"/>
     </row>
-    <row r="41" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
       <c r="B41" s="7"/>
       <c r="C41" s="7"/>
     </row>
-    <row r="42" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="7"/>
       <c r="B42" s="7"/>
       <c r="C42" s="7"/>
     </row>
-    <row r="43" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="7"/>
       <c r="B43" s="7"/>
       <c r="C43" s="7"/>
     </row>
-    <row r="44" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="7"/>
       <c r="B44" s="7"/>
       <c r="C44" s="7"/>
     </row>
-    <row r="45" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="7"/>
       <c r="B45" s="7"/>
       <c r="C45" s="7"/>
     </row>
-    <row r="46" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="7"/>
       <c r="B46" s="7"/>
       <c r="C46" s="7"/>
     </row>
-    <row r="47" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="7"/>
       <c r="B47" s="7"/>
       <c r="C47" s="7"/>
     </row>
-    <row r="48" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="7"/>
       <c r="B48" s="7"/>
       <c r="C48" s="7"/>
     </row>
-    <row r="49" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="7"/>
       <c r="B49" s="7"/>
       <c r="C49" s="7"/>
     </row>
-    <row r="50" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="7"/>
       <c r="B50" s="7"/>
       <c r="C50" s="7"/>
     </row>
-    <row r="51" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="7"/>
       <c r="B51" s="7"/>
       <c r="C51" s="7"/>
     </row>
-    <row r="52" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="7"/>
       <c r="B52" s="7"/>
       <c r="C52" s="7"/>
     </row>
-    <row r="53" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="7"/>
       <c r="B53" s="7"/>
       <c r="C53" s="7"/>
     </row>
-    <row r="54" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="7"/>
       <c r="B54" s="7"/>
       <c r="C54" s="7"/>
     </row>
-    <row r="55" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="7"/>
       <c r="B55" s="7"/>
       <c r="C55" s="7"/>
@@ -1942,20 +1937,41 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
+    <TaxCatchAll xmlns="128482ec-0431-40d5-ab26-89ea2a4f3ccd"/>
+    <m99485b88215436a82099f8287cba0b0 xmlns="128482ec-0431-40d5-ab26-89ea2a4f3ccd">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </m99485b88215436a82099f8287cba0b0>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100723942CCEB3A674D8F1F6472CCEFB38E" ma:contentTypeVersion="3" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="50e7a8f2d4c6c7943ba3cd2d7e94098e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="128482ec-0431-40d5-ab26-89ea2a4f3ccd" xmlns:ns3="60eb0cf4-ae2a-4762-800a-cb593b869ecb" xmlns:ns4="http://schemas.microsoft.com/sharepoint/v4" xmlns:ns5="a2e691a9-fcfc-4d85-a390-1894fe98bd9e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="21625c6912a34b11760d9f0cd1effc5d" ns2:_="" ns3:_="" ns4:_="" ns5:_="">
     <xsd:import namespace="128482ec-0431-40d5-ab26-89ea2a4f3ccd"/>
@@ -2182,35 +2198,42 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
-    <TaxCatchAll xmlns="128482ec-0431-40d5-ab26-89ea2a4f3ccd"/>
-    <m99485b88215436a82099f8287cba0b0 xmlns="128482ec-0431-40d5-ab26-89ea2a4f3ccd">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </m99485b88215436a82099f8287cba0b0>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B7D7A735-0C70-415B-9818-7375747E7F3A}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{25BB2DE4-ECFA-40C6-BD06-2919F1D421BE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
+    <ds:schemaRef ds:uri="128482ec-0431-40d5-ab26-89ea2a4f3ccd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E806665B-1538-472C-8978-66914F77F02C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E806665B-1538-472C-8978-66914F77F02C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{25BB2DE4-ECFA-40C6-BD06-2919F1D421BE}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B7D7A735-0C70-415B-9818-7375747E7F3A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="128482ec-0431-40d5-ab26-89ea2a4f3ccd"/>
+    <ds:schemaRef ds:uri="60eb0cf4-ae2a-4762-800a-cb593b869ecb"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
+    <ds:schemaRef ds:uri="a2e691a9-fcfc-4d85-a390-1894fe98bd9e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>